<commit_message>
- processing Samsung's ServiceProvider file
- upgraded to DevExpress 13.2.6
</commit_message>
<xml_diff>
--- a/Information/LG+Samsung Model Info.xlsx
+++ b/Information/LG+Samsung Model Info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="13395" windowHeight="9270"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="13395" windowHeight="9270" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LG" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="408">
   <si>
     <t>LD</t>
   </si>
@@ -1091,6 +1091,189 @@
   </si>
   <si>
     <t>LK450, LK330</t>
+  </si>
+  <si>
+    <t>Cprime</t>
+  </si>
+  <si>
+    <t>FreeS</t>
+  </si>
+  <si>
+    <t>TivuS</t>
+  </si>
+  <si>
+    <t>PS50C7700</t>
+  </si>
+  <si>
+    <t>ThomasHöhne_CF\channel_list_PS50C7700_1001.scm</t>
+  </si>
+  <si>
+    <t>UE40C6200</t>
+  </si>
+  <si>
+    <t>SamsungBlogNews_20131210\channel_list_UE40C6200_1001.scm</t>
+  </si>
+  <si>
+    <t>UE46C6700</t>
+  </si>
+  <si>
+    <t>C-_und_F-Serie-Favoriten_für_Horst\channel_list_UE46C6700_1001_0103_SL-und-8-Sender-mit-Favoriten.scm</t>
+  </si>
+  <si>
+    <t>LE40D570</t>
+  </si>
+  <si>
+    <t>JHauber_D\channel_list_LE40D570_1101 HD bevorzugt.scm</t>
+  </si>
+  <si>
+    <t>JohannesHauber\channel_list_LE40D570_1101.scm</t>
+  </si>
+  <si>
+    <t>LT27A750</t>
+  </si>
+  <si>
+    <t>Justin\channel_list_LT27A750_1101.scm</t>
+  </si>
+  <si>
+    <t>UE32D5000</t>
+  </si>
+  <si>
+    <t>UMStrehlke\channel_list_UE32D5000_1101.scm</t>
+  </si>
+  <si>
+    <t>UE32D6500</t>
+  </si>
+  <si>
+    <t>ManfredWächtershäuser_D\channel_list_UE32D6500_1101.scm</t>
+  </si>
+  <si>
+    <t>LT24B350</t>
+  </si>
+  <si>
+    <t>DieterHerzberg_B\channel_list_LT24B350_1201.scm</t>
+  </si>
+  <si>
+    <t>LT27C370</t>
+  </si>
+  <si>
+    <t>Anonymous_LT27C370_1201.scm\channel_list_LT27C370_1201.scm</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>Serg0_E\new.scm</t>
+  </si>
+  <si>
+    <t>newer</t>
+  </si>
+  <si>
+    <t>Serg0_E\newer.scm</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Marco - SamsungBlobNews_E\test.scm</t>
+  </si>
+  <si>
+    <t>UE32EH5007</t>
+  </si>
+  <si>
+    <t>Serg0_E\channel_list_UE32EH5007_1201.scm</t>
+  </si>
+  <si>
+    <t>channel_list_UE39F5300_1201\channel_list_UE39F5300_1201.scm</t>
+  </si>
+  <si>
+    <t>UE40F6100</t>
+  </si>
+  <si>
+    <t>RainerSonnenschein_F\channel_list_UE40F6100_1201_org.scm</t>
+  </si>
+  <si>
+    <t>UE40F6500</t>
+  </si>
+  <si>
+    <t>ThomasHöhne_CF\channel_list_UE40F6500_1201.scm</t>
+  </si>
+  <si>
+    <t>Marco - SamsungBlobNews_E\channel_list_UE46ES7000_1201.scm</t>
+  </si>
+  <si>
+    <t>UE46F6500</t>
+  </si>
+  <si>
+    <t>channel_list_UE46F6500_1201_nach_update\channel_list_UE46F6500_1201_nach_update.scm</t>
+  </si>
+  <si>
+    <t>SamsungBlogNews_20131210\channel_list_UE46F6500_1201.scm</t>
+  </si>
+  <si>
+    <t>SamsungBlobNews_F_20131116\channel_list_UE46F6500_1201_vor_update.scm</t>
+  </si>
+  <si>
+    <t>renzullicele_F_tivusat\channel_list_UE46F6500_1201.scm</t>
+  </si>
+  <si>
+    <t>UE46F8000</t>
+  </si>
+  <si>
+    <t>C-_und_F-Serie-Favoriten_für_Horst\channel_list_UE46F8000_1201_0102_SL-und-8-Sender-mit-Favoriten.scm</t>
+  </si>
+  <si>
+    <t>UE55F8000</t>
+  </si>
+  <si>
+    <t>PhilRuelle_F\channel_list_UE55F8000_1201.scm</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>ThomasKotthoff_F\Test.scm</t>
+  </si>
+  <si>
+    <t>Clone_corrected</t>
+  </si>
+  <si>
+    <t>WilliamMoore_B\Clone_corrected.scm</t>
+  </si>
+  <si>
+    <t>Clone_corrected2</t>
+  </si>
+  <si>
+    <t>WilliamMoore_B\Clone_corrected2.scm</t>
+  </si>
+  <si>
+    <t>Clone_downloaded</t>
+  </si>
+  <si>
+    <t>WilliamMoore_B\Clone_downloaded.scm</t>
+  </si>
+  <si>
+    <t>Clone_org</t>
+  </si>
+  <si>
+    <t>WilliamMoore_B\Clone_org.scm</t>
+  </si>
+  <si>
+    <t>Clone_uploaded</t>
+  </si>
+  <si>
+    <t>WilliamMoore_B\Clone_uploaded.scm</t>
+  </si>
+  <si>
+    <t>Clone-AutoScan-Digital</t>
+  </si>
+  <si>
+    <t>Vorher_Nachher\Clone-AutoScan-Digital.scm</t>
+  </si>
+  <si>
+    <t>Clone-DeletedPr2-4</t>
+  </si>
+  <si>
+    <t>Vorher_Nachher\Clone-DeletedPr2-4.scm</t>
   </si>
 </sst>
 </file>
@@ -1480,7 +1663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
     </sheetView>
@@ -6771,11 +6954,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N40"/>
+  <dimension ref="A1:Q71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6791,12 +6974,13 @@
     <col min="9" max="9" width="7" customWidth="1"/>
     <col min="10" max="10" width="6.7109375" customWidth="1"/>
     <col min="11" max="11" width="6.42578125" customWidth="1"/>
-    <col min="12" max="12" width="6.28515625" customWidth="1"/>
-    <col min="13" max="13" width="5.85546875" customWidth="1"/>
-    <col min="14" max="14" width="70.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" customWidth="1"/>
+    <col min="13" max="13" width="6.28515625" customWidth="1"/>
+    <col min="14" max="16" width="5.85546875" customWidth="1"/>
+    <col min="17" max="17" width="70.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:17">
       <c r="A1" s="4" t="s">
         <v>225</v>
       </c>
@@ -6831,13 +7015,22 @@
         <v>224</v>
       </c>
       <c r="L1" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="O1" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>226</v>
       </c>
@@ -6877,16 +7070,25 @@
       <c r="M2">
         <v>0</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>226</v>
       </c>
       <c r="B3" t="s">
-        <v>166</v>
+        <v>394</v>
       </c>
       <c r="C3" s="9">
         <v>28</v>
@@ -6901,7 +7103,7 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>108</v>
+        <v>0</v>
       </c>
       <c r="H3" s="9">
         <v>0</v>
@@ -6913,30 +7115,39 @@
         <v>0</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>499</v>
       </c>
       <c r="L3">
-        <v>1225</v>
+        <v>0</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
-      <c r="N3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>227</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
+        <v>226</v>
+      </c>
+      <c r="B4" t="s">
+        <v>396</v>
       </c>
       <c r="C4" s="9">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D4">
-        <v>292</v>
+        <v>248</v>
       </c>
       <c r="E4">
         <v>144</v>
@@ -6945,19 +7156,19 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>115</v>
+        <v>0</v>
       </c>
       <c r="H4" s="9">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
       <c r="K4">
-        <v>196</v>
+        <v>286</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -6965,22 +7176,31 @@
       <c r="M4">
         <v>0</v>
       </c>
-      <c r="N4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B5" t="s">
-        <v>162</v>
+        <v>398</v>
       </c>
       <c r="C5" s="9">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D5">
-        <v>292</v>
+        <v>248</v>
       </c>
       <c r="E5">
         <v>144</v>
@@ -6989,7 +7209,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>116</v>
+        <v>0</v>
       </c>
       <c r="H5" s="9">
         <v>0</v>
@@ -7001,30 +7221,39 @@
         <v>0</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>499</v>
       </c>
       <c r="L5">
-        <v>1111</v>
+        <v>0</v>
       </c>
       <c r="M5">
         <v>0</v>
       </c>
-      <c r="N5" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B6" t="s">
-        <v>180</v>
+        <v>400</v>
       </c>
       <c r="C6" s="9">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D6">
-        <v>292</v>
+        <v>248</v>
       </c>
       <c r="E6">
         <v>144</v>
@@ -7042,10 +7271,10 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>499</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -7053,22 +7282,31 @@
       <c r="M6">
         <v>0</v>
       </c>
-      <c r="N6" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B7" t="s">
-        <v>180</v>
+        <v>402</v>
       </c>
       <c r="C7" s="9">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D7">
-        <v>292</v>
+        <v>248</v>
       </c>
       <c r="E7">
         <v>144</v>
@@ -7077,7 +7315,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>115</v>
+        <v>0</v>
       </c>
       <c r="H7" s="9">
         <v>0</v>
@@ -7086,10 +7324,10 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>499</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -7097,22 +7335,31 @@
       <c r="M7">
         <v>0</v>
       </c>
-      <c r="N7" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B8" t="s">
-        <v>181</v>
+        <v>404</v>
       </c>
       <c r="C8" s="9">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D8">
-        <v>292</v>
+        <v>248</v>
       </c>
       <c r="E8">
         <v>144</v>
@@ -7133,7 +7380,7 @@
         <v>0</v>
       </c>
       <c r="K8">
-        <v>195</v>
+        <v>499</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -7141,22 +7388,31 @@
       <c r="M8">
         <v>0</v>
       </c>
-      <c r="N8" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B9" t="s">
-        <v>185</v>
+        <v>406</v>
       </c>
       <c r="C9" s="9">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D9">
-        <v>292</v>
+        <v>248</v>
       </c>
       <c r="E9">
         <v>144</v>
@@ -7165,7 +7421,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>116</v>
+        <v>0</v>
       </c>
       <c r="H9" s="9">
         <v>0</v>
@@ -7177,30 +7433,39 @@
         <v>0</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>496</v>
       </c>
       <c r="L9">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
-      <c r="N9" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B10" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="C10" s="9">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D10">
-        <v>292</v>
+        <v>248</v>
       </c>
       <c r="E10">
         <v>144</v>
@@ -7209,13 +7474,13 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H10" s="9">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I10">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -7227,18 +7492,27 @@
         <v>0</v>
       </c>
       <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
+        <v>1225</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
         <v>227</v>
       </c>
-      <c r="B11" t="s">
-        <v>187</v>
+      <c r="B11">
+        <v>1</v>
       </c>
       <c r="C11" s="9">
         <v>40</v>
@@ -7253,19 +7527,19 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H11" s="9">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="I11">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="J11">
         <v>0</v>
       </c>
       <c r="K11">
-        <v>350</v>
+        <v>195</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -7273,16 +7547,25 @@
       <c r="M11">
         <v>0</v>
       </c>
-      <c r="N11" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12" t="s">
         <v>227</v>
       </c>
       <c r="B12" t="s">
-        <v>190</v>
+        <v>162</v>
       </c>
       <c r="C12" s="9">
         <v>40</v>
@@ -7312,21 +7595,30 @@
         <v>0</v>
       </c>
       <c r="L12">
-        <v>227</v>
+        <v>0</v>
       </c>
       <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
+        <v>1111</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13" t="s">
         <v>227</v>
       </c>
       <c r="B13" t="s">
-        <v>233</v>
+        <v>180</v>
       </c>
       <c r="C13" s="9">
         <v>40</v>
@@ -7341,476 +7633,575 @@
         <v>0</v>
       </c>
       <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13" s="9">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>7</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" t="s">
+        <v>227</v>
+      </c>
+      <c r="B14" t="s">
+        <v>180</v>
+      </c>
+      <c r="C14" s="9">
+        <v>40</v>
+      </c>
+      <c r="D14">
+        <v>292</v>
+      </c>
+      <c r="E14">
+        <v>144</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>115</v>
+      </c>
+      <c r="H14" s="9">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>9</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15" t="s">
+        <v>227</v>
+      </c>
+      <c r="B15" t="s">
+        <v>181</v>
+      </c>
+      <c r="C15" s="9">
+        <v>40</v>
+      </c>
+      <c r="D15">
+        <v>292</v>
+      </c>
+      <c r="E15">
+        <v>144</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15" s="9">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>195</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" t="s">
+        <v>227</v>
+      </c>
+      <c r="B16" t="s">
+        <v>185</v>
+      </c>
+      <c r="C16" s="9">
+        <v>40</v>
+      </c>
+      <c r="D16">
+        <v>292</v>
+      </c>
+      <c r="E16">
+        <v>144</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
         <v>116</v>
       </c>
-      <c r="H13" s="9">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
+      <c r="H16" s="9">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>250</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" t="s">
+        <v>227</v>
+      </c>
+      <c r="B17" t="s">
+        <v>350</v>
+      </c>
+      <c r="C17" s="9">
+        <v>40</v>
+      </c>
+      <c r="D17">
+        <v>292</v>
+      </c>
+      <c r="E17">
+        <v>144</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>120</v>
+      </c>
+      <c r="H17" s="9">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>1483</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18" t="s">
+        <v>227</v>
+      </c>
+      <c r="B18" t="s">
+        <v>352</v>
+      </c>
+      <c r="C18" s="9">
+        <v>40</v>
+      </c>
+      <c r="D18">
+        <v>292</v>
+      </c>
+      <c r="E18">
+        <v>144</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>116</v>
+      </c>
+      <c r="H18" s="9">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>1276</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="A19" t="s">
+        <v>227</v>
+      </c>
+      <c r="B19" t="s">
+        <v>187</v>
+      </c>
+      <c r="C19" s="9">
+        <v>40</v>
+      </c>
+      <c r="D19">
+        <v>292</v>
+      </c>
+      <c r="E19">
+        <v>144</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>116</v>
+      </c>
+      <c r="H19" s="9">
+        <v>30</v>
+      </c>
+      <c r="I19">
+        <v>30</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="A20" t="s">
+        <v>227</v>
+      </c>
+      <c r="B20" t="s">
+        <v>187</v>
+      </c>
+      <c r="C20" s="9">
+        <v>40</v>
+      </c>
+      <c r="D20">
+        <v>292</v>
+      </c>
+      <c r="E20">
+        <v>144</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>116</v>
+      </c>
+      <c r="H20" s="9">
+        <v>30</v>
+      </c>
+      <c r="I20">
+        <v>30</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>350</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="A21" t="s">
+        <v>227</v>
+      </c>
+      <c r="B21" t="s">
+        <v>190</v>
+      </c>
+      <c r="C21" s="9">
+        <v>40</v>
+      </c>
+      <c r="D21">
+        <v>292</v>
+      </c>
+      <c r="E21">
+        <v>144</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>116</v>
+      </c>
+      <c r="H21" s="9">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>227</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22" t="s">
+        <v>227</v>
+      </c>
+      <c r="B22" t="s">
+        <v>233</v>
+      </c>
+      <c r="C22" s="9">
+        <v>40</v>
+      </c>
+      <c r="D22">
+        <v>292</v>
+      </c>
+      <c r="E22">
+        <v>144</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>116</v>
+      </c>
+      <c r="H22" s="9">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
         <v>1231</v>
       </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13" t="s">
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
-      <c r="A14" t="s">
+    <row r="23" spans="1:17">
+      <c r="A23" t="s">
+        <v>227</v>
+      </c>
+      <c r="B23" t="s">
+        <v>354</v>
+      </c>
+      <c r="C23" s="9">
+        <v>40</v>
+      </c>
+      <c r="D23">
+        <v>292</v>
+      </c>
+      <c r="E23">
+        <v>144</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>116</v>
+      </c>
+      <c r="H23" s="9">
+        <v>38</v>
+      </c>
+      <c r="I23">
+        <v>38</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>497</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="A24" t="s">
         <v>228</v>
       </c>
-      <c r="B14" t="s">
-        <v>164</v>
-      </c>
-      <c r="C14" s="9">
-        <v>64</v>
-      </c>
-      <c r="D14">
-        <v>320</v>
-      </c>
-      <c r="E14">
-        <v>172</v>
-      </c>
-      <c r="F14">
-        <v>212</v>
-      </c>
-      <c r="G14">
-        <v>129</v>
-      </c>
-      <c r="H14" s="9">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14">
-        <v>1222</v>
-      </c>
-      <c r="M14">
-        <v>731</v>
-      </c>
-      <c r="N14" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="A15" t="s">
-        <v>228</v>
-      </c>
-      <c r="B15" t="s">
-        <v>170</v>
-      </c>
-      <c r="C15" s="9">
-        <v>64</v>
-      </c>
-      <c r="D15">
-        <v>320</v>
-      </c>
-      <c r="E15">
-        <v>172</v>
-      </c>
-      <c r="F15">
-        <v>212</v>
-      </c>
-      <c r="G15">
-        <v>129</v>
-      </c>
-      <c r="H15" s="9">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>11</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <v>210</v>
-      </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="A16" t="s">
-        <v>228</v>
-      </c>
-      <c r="B16" t="s">
-        <v>176</v>
-      </c>
-      <c r="C16" s="9">
-        <v>64</v>
-      </c>
-      <c r="D16">
-        <v>320</v>
-      </c>
-      <c r="E16">
-        <v>172</v>
-      </c>
-      <c r="F16">
-        <v>212</v>
-      </c>
-      <c r="G16">
-        <v>126</v>
-      </c>
-      <c r="H16" s="9">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <v>15</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <v>550</v>
-      </c>
-      <c r="M16">
-        <v>0</v>
-      </c>
-      <c r="N16" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
-      <c r="A17" t="s">
-        <v>228</v>
-      </c>
-      <c r="B17" t="s">
-        <v>178</v>
-      </c>
-      <c r="C17" s="9">
-        <v>64</v>
-      </c>
-      <c r="D17">
-        <v>320</v>
-      </c>
-      <c r="E17">
-        <v>172</v>
-      </c>
-      <c r="F17">
-        <v>212</v>
-      </c>
-      <c r="G17">
-        <v>129</v>
-      </c>
-      <c r="H17" s="9">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17">
-        <v>577</v>
-      </c>
-      <c r="N17" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14">
-      <c r="A18" t="s">
-        <v>228</v>
-      </c>
-      <c r="B18" t="s">
-        <v>183</v>
-      </c>
-      <c r="C18" s="9">
-        <v>64</v>
-      </c>
-      <c r="D18">
-        <v>320</v>
-      </c>
-      <c r="E18">
-        <v>172</v>
-      </c>
-      <c r="F18">
-        <v>212</v>
-      </c>
-      <c r="G18">
-        <v>129</v>
-      </c>
-      <c r="H18" s="9">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>1078</v>
-      </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="N18" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14">
-      <c r="A19" t="s">
-        <v>228</v>
-      </c>
-      <c r="B19" t="s">
-        <v>192</v>
-      </c>
-      <c r="C19" s="9">
-        <v>64</v>
-      </c>
-      <c r="D19">
-        <v>320</v>
-      </c>
-      <c r="E19">
-        <v>172</v>
-      </c>
-      <c r="F19">
-        <v>212</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19" s="9">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
-      <c r="K19">
-        <v>454</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-      <c r="N19" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
-      <c r="A20" t="s">
-        <v>228</v>
-      </c>
-      <c r="B20" t="s">
-        <v>194</v>
-      </c>
-      <c r="C20" s="9">
-        <v>64</v>
-      </c>
-      <c r="D20">
-        <v>320</v>
-      </c>
-      <c r="E20">
-        <v>172</v>
-      </c>
-      <c r="F20">
-        <v>212</v>
-      </c>
-      <c r="G20">
-        <v>129</v>
-      </c>
-      <c r="H20" s="9">
-        <v>32</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
-      <c r="N20" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="A21" t="s">
-        <v>228</v>
-      </c>
-      <c r="B21" t="s">
-        <v>206</v>
-      </c>
-      <c r="C21" s="9">
-        <v>64</v>
-      </c>
-      <c r="D21">
-        <v>320</v>
-      </c>
-      <c r="E21">
-        <v>172</v>
-      </c>
-      <c r="F21">
-        <v>212</v>
-      </c>
-      <c r="G21">
-        <v>129</v>
-      </c>
-      <c r="H21" s="9">
-        <v>74</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <v>71</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="M21">
-        <v>0</v>
-      </c>
-      <c r="N21" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14">
-      <c r="A22" t="s">
-        <v>229</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="B24" t="s">
         <v>156</v>
-      </c>
-      <c r="C22" s="9">
-        <v>64</v>
-      </c>
-      <c r="D22">
-        <v>320</v>
-      </c>
-      <c r="E22">
-        <v>168</v>
-      </c>
-      <c r="F22">
-        <v>212</v>
-      </c>
-      <c r="G22">
-        <v>131</v>
-      </c>
-      <c r="H22" s="9">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
-        <v>123</v>
-      </c>
-      <c r="M22">
-        <v>0</v>
-      </c>
-      <c r="N22" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14">
-      <c r="A23" t="s">
-        <v>229</v>
-      </c>
-      <c r="B23" t="s">
-        <v>158</v>
-      </c>
-      <c r="C23" s="9">
-        <v>64</v>
-      </c>
-      <c r="D23">
-        <v>320</v>
-      </c>
-      <c r="E23">
-        <v>168</v>
-      </c>
-      <c r="F23">
-        <v>212</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23" s="9">
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-      <c r="K23">
-        <v>423</v>
-      </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-      <c r="M23">
-        <v>0</v>
-      </c>
-      <c r="N23" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14">
-      <c r="A24" t="s">
-        <v>229</v>
-      </c>
-      <c r="B24" t="s">
-        <v>168</v>
       </c>
       <c r="C24" s="9">
         <v>64</v>
@@ -7819,13 +8210,13 @@
         <v>320</v>
       </c>
       <c r="E24">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="F24">
         <v>212</v>
       </c>
       <c r="G24">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="H24" s="9">
         <v>0</v>
@@ -7840,21 +8231,30 @@
         <v>0</v>
       </c>
       <c r="L24">
-        <v>1274</v>
+        <v>0</v>
       </c>
       <c r="M24">
-        <v>744</v>
-      </c>
-      <c r="N24" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14">
+        <v>553</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
       <c r="A25" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B25" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="C25" s="9">
         <v>64</v>
@@ -7863,13 +8263,13 @@
         <v>320</v>
       </c>
       <c r="E25">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="F25">
         <v>212</v>
       </c>
       <c r="G25">
-        <v>151</v>
+        <v>129</v>
       </c>
       <c r="H25" s="9">
         <v>0</v>
@@ -7878,27 +8278,36 @@
         <v>0</v>
       </c>
       <c r="J25">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="K25">
         <v>0</v>
       </c>
       <c r="L25">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="M25">
-        <v>0</v>
-      </c>
-      <c r="N25" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14">
+        <v>1222</v>
+      </c>
+      <c r="N25">
+        <v>731</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
       <c r="A26" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B26" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C26" s="9">
         <v>64</v>
@@ -7907,13 +8316,13 @@
         <v>320</v>
       </c>
       <c r="E26">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="F26">
         <v>212</v>
       </c>
       <c r="G26">
-        <v>151</v>
+        <v>129</v>
       </c>
       <c r="H26" s="9">
         <v>0</v>
@@ -7928,21 +8337,30 @@
         <v>0</v>
       </c>
       <c r="L26">
-        <v>585</v>
+        <v>0</v>
       </c>
       <c r="M26">
-        <v>0</v>
-      </c>
-      <c r="N26" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14">
+        <v>210</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
       <c r="A27" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B27" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="C27" s="9">
         <v>64</v>
@@ -7951,42 +8369,51 @@
         <v>320</v>
       </c>
       <c r="E27">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="F27">
         <v>212</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>126</v>
       </c>
       <c r="H27" s="9">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="I27">
         <v>0</v>
       </c>
       <c r="J27">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="K27">
-        <v>461</v>
+        <v>0</v>
       </c>
       <c r="L27">
         <v>0</v>
       </c>
       <c r="M27">
-        <v>0</v>
-      </c>
-      <c r="N27" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14">
+        <v>550</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
       <c r="A28" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B28" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
       <c r="C28" s="9">
         <v>64</v>
@@ -7995,13 +8422,13 @@
         <v>320</v>
       </c>
       <c r="E28">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="F28">
         <v>212</v>
       </c>
       <c r="G28">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="H28" s="9">
         <v>0</v>
@@ -8016,21 +8443,30 @@
         <v>0</v>
       </c>
       <c r="L28">
-        <v>2361</v>
+        <v>0</v>
       </c>
       <c r="M28">
         <v>0</v>
       </c>
-      <c r="N28" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14">
+      <c r="N28">
+        <v>577</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
       <c r="A29" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B29" t="s">
-        <v>200</v>
+        <v>356</v>
       </c>
       <c r="C29" s="9">
         <v>64</v>
@@ -8039,13 +8475,13 @@
         <v>320</v>
       </c>
       <c r="E29">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="F29">
         <v>212</v>
       </c>
       <c r="G29">
-        <v>151</v>
+        <v>131</v>
       </c>
       <c r="H29" s="9">
         <v>0</v>
@@ -8060,21 +8496,30 @@
         <v>0</v>
       </c>
       <c r="L29">
-        <v>1940</v>
+        <v>0</v>
       </c>
       <c r="M29">
         <v>0</v>
       </c>
-      <c r="N29" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14">
+      <c r="N29">
+        <v>721</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <v>0</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
       <c r="A30" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B30" t="s">
-        <v>208</v>
+        <v>356</v>
       </c>
       <c r="C30" s="9">
         <v>64</v>
@@ -8083,16 +8528,16 @@
         <v>320</v>
       </c>
       <c r="E30">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="F30">
         <v>212</v>
       </c>
       <c r="G30">
-        <v>151</v>
+        <v>131</v>
       </c>
       <c r="H30" s="9">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I30">
         <v>0</v>
@@ -8101,24 +8546,33 @@
         <v>0</v>
       </c>
       <c r="K30">
-        <v>363</v>
+        <v>0</v>
       </c>
       <c r="L30">
         <v>0</v>
       </c>
       <c r="M30">
-        <v>680</v>
-      </c>
-      <c r="N30" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14">
+        <v>951</v>
+      </c>
+      <c r="N30">
+        <v>717</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <v>0</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
       <c r="A31" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B31" t="s">
-        <v>210</v>
+        <v>359</v>
       </c>
       <c r="C31" s="9">
         <v>64</v>
@@ -8127,13 +8581,13 @@
         <v>320</v>
       </c>
       <c r="E31">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="F31">
         <v>212</v>
       </c>
       <c r="G31">
-        <v>151</v>
+        <v>0</v>
       </c>
       <c r="H31" s="9">
         <v>0</v>
@@ -8142,27 +8596,36 @@
         <v>0</v>
       </c>
       <c r="J31">
-        <v>0</v>
+        <v>214</v>
       </c>
       <c r="K31">
         <v>0</v>
       </c>
       <c r="L31">
-        <v>1940</v>
+        <v>0</v>
       </c>
       <c r="M31">
         <v>0</v>
       </c>
-      <c r="N31" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14">
+      <c r="N31">
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <v>0</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
       <c r="A32" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B32" t="s">
-        <v>212</v>
+        <v>183</v>
       </c>
       <c r="C32" s="9">
         <v>64</v>
@@ -8171,13 +8634,13 @@
         <v>320</v>
       </c>
       <c r="E32">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="F32">
         <v>212</v>
       </c>
       <c r="G32">
-        <v>151</v>
+        <v>129</v>
       </c>
       <c r="H32" s="9">
         <v>0</v>
@@ -8192,21 +8655,30 @@
         <v>0</v>
       </c>
       <c r="L32">
-        <v>1274</v>
+        <v>0</v>
       </c>
       <c r="M32">
-        <v>753</v>
-      </c>
-      <c r="N32" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14">
+        <v>1078</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <v>0</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17">
       <c r="A33" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B33" t="s">
-        <v>214</v>
+        <v>361</v>
       </c>
       <c r="C33" s="9">
         <v>64</v>
@@ -8215,7 +8687,7 @@
         <v>320</v>
       </c>
       <c r="E33">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="F33">
         <v>212</v>
@@ -8224,7 +8696,7 @@
         <v>0</v>
       </c>
       <c r="H33" s="9">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="I33">
         <v>0</v>
@@ -8233,7 +8705,7 @@
         <v>0</v>
       </c>
       <c r="K33">
-        <v>532</v>
+        <v>149</v>
       </c>
       <c r="L33">
         <v>0</v>
@@ -8241,16 +8713,25 @@
       <c r="M33">
         <v>0</v>
       </c>
-      <c r="N33" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14">
+      <c r="N33">
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <v>0</v>
+      </c>
+      <c r="P33">
+        <v>0</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17">
       <c r="A34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B34" t="s">
-        <v>235</v>
+        <v>363</v>
       </c>
       <c r="C34" s="9">
         <v>64</v>
@@ -8259,22 +8740,22 @@
         <v>320</v>
       </c>
       <c r="E34">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="F34">
         <v>212</v>
       </c>
       <c r="G34">
-        <v>159</v>
+        <v>131</v>
       </c>
       <c r="H34" s="9">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="I34">
         <v>0</v>
       </c>
       <c r="J34">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="K34">
         <v>0</v>
@@ -8285,16 +8766,25 @@
       <c r="M34">
         <v>0</v>
       </c>
-      <c r="N34" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14">
+      <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <v>0</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17">
       <c r="A35" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B35" t="s">
-        <v>237</v>
+        <v>192</v>
       </c>
       <c r="C35" s="9">
         <v>64</v>
@@ -8303,13 +8793,13 @@
         <v>320</v>
       </c>
       <c r="E35">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="F35">
         <v>212</v>
       </c>
       <c r="G35">
-        <v>159</v>
+        <v>0</v>
       </c>
       <c r="H35" s="9">
         <v>0</v>
@@ -8321,24 +8811,33 @@
         <v>0</v>
       </c>
       <c r="K35">
-        <v>0</v>
+        <v>454</v>
       </c>
       <c r="L35">
         <v>0</v>
       </c>
       <c r="M35">
-        <v>50</v>
-      </c>
-      <c r="N35" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <v>0</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17">
       <c r="A36" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B36" t="s">
-        <v>239</v>
+        <v>194</v>
       </c>
       <c r="C36" s="9">
         <v>64</v>
@@ -8347,16 +8846,16 @@
         <v>320</v>
       </c>
       <c r="E36">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="F36">
         <v>212</v>
       </c>
       <c r="G36">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="H36" s="9">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="I36">
         <v>0</v>
@@ -8371,18 +8870,27 @@
         <v>0</v>
       </c>
       <c r="M36">
-        <v>761</v>
-      </c>
-      <c r="N36" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14">
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <v>0</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="P36">
+        <v>0</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17">
       <c r="A37" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B37" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="C37" s="9">
         <v>64</v>
@@ -8391,16 +8899,16 @@
         <v>320</v>
       </c>
       <c r="E37">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="F37">
         <v>212</v>
       </c>
       <c r="G37">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="H37" s="9">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="I37">
         <v>0</v>
@@ -8409,7 +8917,7 @@
         <v>0</v>
       </c>
       <c r="K37">
-        <v>290</v>
+        <v>71</v>
       </c>
       <c r="L37">
         <v>0</v>
@@ -8417,16 +8925,25 @@
       <c r="M37">
         <v>0</v>
       </c>
-      <c r="N37" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14">
+      <c r="N37">
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="P37">
+        <v>0</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17">
       <c r="A38" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B38" t="s">
-        <v>204</v>
+        <v>158</v>
       </c>
       <c r="C38" s="9">
         <v>64</v>
@@ -8441,36 +8958,45 @@
         <v>212</v>
       </c>
       <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38" s="9">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <v>423</v>
+      </c>
+      <c r="L38">
+        <v>0</v>
+      </c>
+      <c r="M38">
+        <v>0</v>
+      </c>
+      <c r="N38">
+        <v>0</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
+      </c>
+      <c r="P38">
+        <v>0</v>
+      </c>
+      <c r="Q38" t="s">
         <v>159</v>
       </c>
-      <c r="H38" s="9">
-        <v>37</v>
-      </c>
-      <c r="I38">
-        <v>0</v>
-      </c>
-      <c r="J38">
-        <v>0</v>
-      </c>
-      <c r="K38">
-        <v>533</v>
-      </c>
-      <c r="L38">
-        <v>0</v>
-      </c>
-      <c r="M38">
-        <v>0</v>
-      </c>
-      <c r="N38" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14">
+    </row>
+    <row r="39" spans="1:17">
       <c r="A39" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B39" t="s">
-        <v>216</v>
+        <v>168</v>
       </c>
       <c r="C39" s="9">
         <v>64</v>
@@ -8485,7 +9011,7 @@
         <v>212</v>
       </c>
       <c r="G39">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="H39" s="9">
         <v>0</v>
@@ -8500,21 +9026,30 @@
         <v>0</v>
       </c>
       <c r="L39">
-        <v>221</v>
+        <v>0</v>
       </c>
       <c r="M39">
-        <v>0</v>
-      </c>
-      <c r="N39" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14">
+        <v>1274</v>
+      </c>
+      <c r="N39">
+        <v>744</v>
+      </c>
+      <c r="O39">
+        <v>0</v>
+      </c>
+      <c r="P39">
+        <v>0</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17">
       <c r="A40" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B40" t="s">
-        <v>216</v>
+        <v>172</v>
       </c>
       <c r="C40" s="9">
         <v>64</v>
@@ -8529,28 +9064,1680 @@
         <v>212</v>
       </c>
       <c r="G40">
+        <v>151</v>
+      </c>
+      <c r="H40" s="9">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>37</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <v>49</v>
+      </c>
+      <c r="N40">
+        <v>0</v>
+      </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+      <c r="P40">
+        <v>0</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17">
+      <c r="A41" t="s">
+        <v>229</v>
+      </c>
+      <c r="B41" t="s">
+        <v>174</v>
+      </c>
+      <c r="C41" s="9">
+        <v>64</v>
+      </c>
+      <c r="D41">
+        <v>320</v>
+      </c>
+      <c r="E41">
+        <v>168</v>
+      </c>
+      <c r="F41">
+        <v>212</v>
+      </c>
+      <c r="G41">
+        <v>151</v>
+      </c>
+      <c r="H41" s="9">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>11</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
+      <c r="M41">
+        <v>585</v>
+      </c>
+      <c r="N41">
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <v>0</v>
+      </c>
+      <c r="P41">
+        <v>0</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17">
+      <c r="A42" t="s">
+        <v>229</v>
+      </c>
+      <c r="B42" t="s">
+        <v>365</v>
+      </c>
+      <c r="C42" s="9">
+        <v>64</v>
+      </c>
+      <c r="D42">
+        <v>320</v>
+      </c>
+      <c r="E42">
+        <v>168</v>
+      </c>
+      <c r="F42">
+        <v>212</v>
+      </c>
+      <c r="G42">
+        <v>140</v>
+      </c>
+      <c r="H42" s="9">
+        <v>32</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>17</v>
+      </c>
+      <c r="K42">
+        <v>395</v>
+      </c>
+      <c r="L42">
+        <v>0</v>
+      </c>
+      <c r="M42">
+        <v>0</v>
+      </c>
+      <c r="N42">
+        <v>0</v>
+      </c>
+      <c r="O42">
+        <v>0</v>
+      </c>
+      <c r="P42">
+        <v>0</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17">
+      <c r="A43" t="s">
+        <v>229</v>
+      </c>
+      <c r="B43" t="s">
+        <v>367</v>
+      </c>
+      <c r="C43" s="9">
+        <v>64</v>
+      </c>
+      <c r="D43">
+        <v>320</v>
+      </c>
+      <c r="E43">
+        <v>168</v>
+      </c>
+      <c r="F43">
+        <v>212</v>
+      </c>
+      <c r="G43">
+        <v>151</v>
+      </c>
+      <c r="H43" s="9">
+        <v>30</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>395</v>
+      </c>
+      <c r="L43">
+        <v>0</v>
+      </c>
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43">
+        <v>0</v>
+      </c>
+      <c r="O43">
+        <v>0</v>
+      </c>
+      <c r="P43">
+        <v>0</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17">
+      <c r="A44" t="s">
+        <v>229</v>
+      </c>
+      <c r="B44" t="s">
+        <v>369</v>
+      </c>
+      <c r="C44" s="9">
+        <v>64</v>
+      </c>
+      <c r="D44">
+        <v>320</v>
+      </c>
+      <c r="E44">
+        <v>168</v>
+      </c>
+      <c r="F44">
+        <v>212</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44" s="9">
+        <v>69</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
+      <c r="L44">
+        <v>0</v>
+      </c>
+      <c r="M44">
+        <v>0</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <v>0</v>
+      </c>
+      <c r="P44">
+        <v>0</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17">
+      <c r="A45" t="s">
+        <v>229</v>
+      </c>
+      <c r="B45" t="s">
+        <v>371</v>
+      </c>
+      <c r="C45" s="9">
+        <v>64</v>
+      </c>
+      <c r="D45">
+        <v>320</v>
+      </c>
+      <c r="E45">
+        <v>168</v>
+      </c>
+      <c r="F45">
+        <v>212</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45" s="9">
+        <v>69</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+      <c r="L45">
+        <v>0</v>
+      </c>
+      <c r="M45">
+        <v>0</v>
+      </c>
+      <c r="N45">
+        <v>0</v>
+      </c>
+      <c r="O45">
+        <v>0</v>
+      </c>
+      <c r="P45">
+        <v>0</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17">
+      <c r="A46" t="s">
+        <v>229</v>
+      </c>
+      <c r="B46" t="s">
+        <v>373</v>
+      </c>
+      <c r="C46" s="9">
+        <v>64</v>
+      </c>
+      <c r="D46">
+        <v>320</v>
+      </c>
+      <c r="E46">
+        <v>168</v>
+      </c>
+      <c r="F46">
+        <v>212</v>
+      </c>
+      <c r="G46">
         <v>159</v>
       </c>
-      <c r="H40" s="9">
-        <v>0</v>
-      </c>
-      <c r="I40">
-        <v>0</v>
-      </c>
-      <c r="J40">
-        <v>0</v>
-      </c>
-      <c r="K40">
-        <v>0</v>
-      </c>
-      <c r="L40">
+      <c r="H46" s="9">
+        <v>34</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>0</v>
+      </c>
+      <c r="L46">
+        <v>8</v>
+      </c>
+      <c r="M46">
+        <v>0</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
+      <c r="O46">
+        <v>0</v>
+      </c>
+      <c r="P46">
+        <v>0</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17">
+      <c r="A47" t="s">
+        <v>229</v>
+      </c>
+      <c r="B47" t="s">
+        <v>375</v>
+      </c>
+      <c r="C47" s="9">
+        <v>64</v>
+      </c>
+      <c r="D47">
+        <v>320</v>
+      </c>
+      <c r="E47">
+        <v>168</v>
+      </c>
+      <c r="F47">
+        <v>212</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47" s="9">
+        <v>69</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>159</v>
+      </c>
+      <c r="L47">
+        <v>0</v>
+      </c>
+      <c r="M47">
+        <v>0</v>
+      </c>
+      <c r="N47">
+        <v>0</v>
+      </c>
+      <c r="O47">
+        <v>0</v>
+      </c>
+      <c r="P47">
+        <v>0</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17">
+      <c r="A48" t="s">
+        <v>229</v>
+      </c>
+      <c r="B48" t="s">
+        <v>196</v>
+      </c>
+      <c r="C48" s="9">
+        <v>64</v>
+      </c>
+      <c r="D48">
+        <v>320</v>
+      </c>
+      <c r="E48">
+        <v>168</v>
+      </c>
+      <c r="F48">
+        <v>212</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48" s="9">
+        <v>34</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>461</v>
+      </c>
+      <c r="L48">
+        <v>0</v>
+      </c>
+      <c r="M48">
+        <v>0</v>
+      </c>
+      <c r="N48">
+        <v>0</v>
+      </c>
+      <c r="O48">
+        <v>0</v>
+      </c>
+      <c r="P48">
+        <v>0</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17">
+      <c r="A49" t="s">
+        <v>229</v>
+      </c>
+      <c r="B49" t="s">
+        <v>198</v>
+      </c>
+      <c r="C49" s="9">
+        <v>64</v>
+      </c>
+      <c r="D49">
+        <v>320</v>
+      </c>
+      <c r="E49">
+        <v>168</v>
+      </c>
+      <c r="F49">
+        <v>212</v>
+      </c>
+      <c r="G49">
+        <v>147</v>
+      </c>
+      <c r="H49" s="9">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+      <c r="M49">
+        <v>2361</v>
+      </c>
+      <c r="N49">
+        <v>0</v>
+      </c>
+      <c r="O49">
+        <v>0</v>
+      </c>
+      <c r="P49">
+        <v>0</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17">
+      <c r="A50" t="s">
+        <v>229</v>
+      </c>
+      <c r="B50" t="s">
+        <v>200</v>
+      </c>
+      <c r="C50" s="9">
+        <v>64</v>
+      </c>
+      <c r="D50">
+        <v>320</v>
+      </c>
+      <c r="E50">
+        <v>168</v>
+      </c>
+      <c r="F50">
+        <v>212</v>
+      </c>
+      <c r="G50">
+        <v>151</v>
+      </c>
+      <c r="H50" s="9">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>0</v>
+      </c>
+      <c r="L50">
+        <v>0</v>
+      </c>
+      <c r="M50">
+        <v>1940</v>
+      </c>
+      <c r="N50">
+        <v>0</v>
+      </c>
+      <c r="O50">
+        <v>0</v>
+      </c>
+      <c r="P50">
+        <v>0</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17">
+      <c r="A51" t="s">
+        <v>229</v>
+      </c>
+      <c r="B51" t="s">
+        <v>208</v>
+      </c>
+      <c r="C51" s="9">
+        <v>64</v>
+      </c>
+      <c r="D51">
+        <v>320</v>
+      </c>
+      <c r="E51">
+        <v>168</v>
+      </c>
+      <c r="F51">
+        <v>212</v>
+      </c>
+      <c r="G51">
+        <v>151</v>
+      </c>
+      <c r="H51" s="9">
+        <v>30</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51">
+        <v>0</v>
+      </c>
+      <c r="K51">
+        <v>363</v>
+      </c>
+      <c r="L51">
+        <v>0</v>
+      </c>
+      <c r="M51">
+        <v>0</v>
+      </c>
+      <c r="N51">
+        <v>680</v>
+      </c>
+      <c r="O51">
+        <v>0</v>
+      </c>
+      <c r="P51">
+        <v>0</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17">
+      <c r="A52" t="s">
+        <v>229</v>
+      </c>
+      <c r="B52" t="s">
+        <v>210</v>
+      </c>
+      <c r="C52" s="9">
+        <v>64</v>
+      </c>
+      <c r="D52">
+        <v>320</v>
+      </c>
+      <c r="E52">
+        <v>168</v>
+      </c>
+      <c r="F52">
+        <v>212</v>
+      </c>
+      <c r="G52">
+        <v>151</v>
+      </c>
+      <c r="H52" s="9">
+        <v>0</v>
+      </c>
+      <c r="I52">
+        <v>0</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+      <c r="K52">
+        <v>0</v>
+      </c>
+      <c r="L52">
+        <v>0</v>
+      </c>
+      <c r="M52">
+        <v>1940</v>
+      </c>
+      <c r="N52">
+        <v>0</v>
+      </c>
+      <c r="O52">
+        <v>0</v>
+      </c>
+      <c r="P52">
+        <v>0</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17">
+      <c r="A53" t="s">
+        <v>229</v>
+      </c>
+      <c r="B53" t="s">
+        <v>212</v>
+      </c>
+      <c r="C53" s="9">
+        <v>64</v>
+      </c>
+      <c r="D53">
+        <v>320</v>
+      </c>
+      <c r="E53">
+        <v>168</v>
+      </c>
+      <c r="F53">
+        <v>212</v>
+      </c>
+      <c r="G53">
+        <v>151</v>
+      </c>
+      <c r="H53" s="9">
+        <v>0</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <v>0</v>
+      </c>
+      <c r="K53">
+        <v>0</v>
+      </c>
+      <c r="L53">
+        <v>0</v>
+      </c>
+      <c r="M53">
+        <v>1274</v>
+      </c>
+      <c r="N53">
+        <v>753</v>
+      </c>
+      <c r="O53">
+        <v>0</v>
+      </c>
+      <c r="P53">
+        <v>0</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17">
+      <c r="A54" t="s">
+        <v>229</v>
+      </c>
+      <c r="B54" t="s">
+        <v>212</v>
+      </c>
+      <c r="C54" s="9">
+        <v>64</v>
+      </c>
+      <c r="D54">
+        <v>320</v>
+      </c>
+      <c r="E54">
+        <v>168</v>
+      </c>
+      <c r="F54">
+        <v>212</v>
+      </c>
+      <c r="G54">
+        <v>159</v>
+      </c>
+      <c r="H54" s="9">
+        <v>34</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <v>0</v>
+      </c>
+      <c r="L54">
+        <v>466</v>
+      </c>
+      <c r="M54">
+        <v>0</v>
+      </c>
+      <c r="N54">
+        <v>0</v>
+      </c>
+      <c r="O54">
+        <v>0</v>
+      </c>
+      <c r="P54">
+        <v>0</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17">
+      <c r="A55" t="s">
+        <v>229</v>
+      </c>
+      <c r="B55" t="s">
+        <v>214</v>
+      </c>
+      <c r="C55" s="9">
+        <v>64</v>
+      </c>
+      <c r="D55">
+        <v>320</v>
+      </c>
+      <c r="E55">
+        <v>168</v>
+      </c>
+      <c r="F55">
+        <v>212</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55" s="9">
+        <v>37</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+      <c r="K55">
+        <v>532</v>
+      </c>
+      <c r="L55">
+        <v>0</v>
+      </c>
+      <c r="M55">
+        <v>0</v>
+      </c>
+      <c r="N55">
+        <v>0</v>
+      </c>
+      <c r="O55">
+        <v>0</v>
+      </c>
+      <c r="P55">
+        <v>0</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17">
+      <c r="A56" t="s">
+        <v>229</v>
+      </c>
+      <c r="B56" t="s">
+        <v>235</v>
+      </c>
+      <c r="C56" s="9">
+        <v>64</v>
+      </c>
+      <c r="D56">
+        <v>320</v>
+      </c>
+      <c r="E56">
+        <v>168</v>
+      </c>
+      <c r="F56">
+        <v>212</v>
+      </c>
+      <c r="G56">
+        <v>159</v>
+      </c>
+      <c r="H56" s="9">
+        <v>32</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <v>0</v>
+      </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
+      <c r="L56">
+        <v>385</v>
+      </c>
+      <c r="M56">
+        <v>0</v>
+      </c>
+      <c r="N56">
+        <v>0</v>
+      </c>
+      <c r="O56">
+        <v>0</v>
+      </c>
+      <c r="P56">
+        <v>0</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17">
+      <c r="A57" t="s">
+        <v>230</v>
+      </c>
+      <c r="B57" t="s">
+        <v>392</v>
+      </c>
+      <c r="C57" s="9">
+        <v>64</v>
+      </c>
+      <c r="D57">
+        <v>320</v>
+      </c>
+      <c r="E57">
+        <v>168</v>
+      </c>
+      <c r="F57">
+        <v>212</v>
+      </c>
+      <c r="G57">
+        <v>159</v>
+      </c>
+      <c r="H57" s="9">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57">
+        <v>0</v>
+      </c>
+      <c r="K57">
+        <v>0</v>
+      </c>
+      <c r="L57">
+        <v>0</v>
+      </c>
+      <c r="M57">
+        <v>0</v>
+      </c>
+      <c r="N57">
+        <v>701</v>
+      </c>
+      <c r="O57">
+        <v>0</v>
+      </c>
+      <c r="P57">
+        <v>0</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17">
+      <c r="A58" t="s">
+        <v>230</v>
+      </c>
+      <c r="B58" t="s">
+        <v>237</v>
+      </c>
+      <c r="C58" s="9">
+        <v>64</v>
+      </c>
+      <c r="D58">
+        <v>320</v>
+      </c>
+      <c r="E58">
+        <v>168</v>
+      </c>
+      <c r="F58">
+        <v>212</v>
+      </c>
+      <c r="G58">
+        <v>159</v>
+      </c>
+      <c r="H58" s="9">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58">
+        <v>0</v>
+      </c>
+      <c r="K58">
+        <v>0</v>
+      </c>
+      <c r="L58">
+        <v>0</v>
+      </c>
+      <c r="M58">
+        <v>0</v>
+      </c>
+      <c r="N58">
+        <v>0</v>
+      </c>
+      <c r="O58">
+        <v>0</v>
+      </c>
+      <c r="P58">
+        <v>0</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17">
+      <c r="A59" t="s">
+        <v>230</v>
+      </c>
+      <c r="B59" t="s">
+        <v>237</v>
+      </c>
+      <c r="C59" s="9">
+        <v>64</v>
+      </c>
+      <c r="D59">
+        <v>320</v>
+      </c>
+      <c r="E59">
+        <v>168</v>
+      </c>
+      <c r="F59">
+        <v>212</v>
+      </c>
+      <c r="G59">
+        <v>159</v>
+      </c>
+      <c r="H59" s="9">
+        <v>0</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
+      <c r="J59">
+        <v>0</v>
+      </c>
+      <c r="K59">
+        <v>0</v>
+      </c>
+      <c r="L59">
+        <v>0</v>
+      </c>
+      <c r="M59">
+        <v>0</v>
+      </c>
+      <c r="N59">
+        <v>50</v>
+      </c>
+      <c r="O59">
+        <v>0</v>
+      </c>
+      <c r="P59">
+        <v>0</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17">
+      <c r="A60" t="s">
+        <v>230</v>
+      </c>
+      <c r="B60" t="s">
+        <v>239</v>
+      </c>
+      <c r="C60" s="9">
+        <v>64</v>
+      </c>
+      <c r="D60">
+        <v>320</v>
+      </c>
+      <c r="E60">
+        <v>168</v>
+      </c>
+      <c r="F60">
+        <v>212</v>
+      </c>
+      <c r="G60">
+        <v>159</v>
+      </c>
+      <c r="H60" s="9">
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="J60">
+        <v>0</v>
+      </c>
+      <c r="K60">
+        <v>0</v>
+      </c>
+      <c r="L60">
+        <v>0</v>
+      </c>
+      <c r="M60">
+        <v>0</v>
+      </c>
+      <c r="N60">
+        <v>761</v>
+      </c>
+      <c r="O60">
+        <v>0</v>
+      </c>
+      <c r="P60">
+        <v>0</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17">
+      <c r="A61" t="s">
+        <v>230</v>
+      </c>
+      <c r="B61" t="s">
+        <v>378</v>
+      </c>
+      <c r="C61" s="9">
+        <v>64</v>
+      </c>
+      <c r="D61">
+        <v>320</v>
+      </c>
+      <c r="E61">
+        <v>168</v>
+      </c>
+      <c r="F61">
+        <v>212</v>
+      </c>
+      <c r="G61">
+        <v>159</v>
+      </c>
+      <c r="H61" s="9">
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <v>44</v>
+      </c>
+      <c r="K61">
+        <v>229</v>
+      </c>
+      <c r="L61">
+        <v>0</v>
+      </c>
+      <c r="M61">
+        <v>0</v>
+      </c>
+      <c r="N61">
+        <v>0</v>
+      </c>
+      <c r="O61">
+        <v>0</v>
+      </c>
+      <c r="P61">
+        <v>0</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17">
+      <c r="A62" t="s">
+        <v>230</v>
+      </c>
+      <c r="B62" t="s">
+        <v>380</v>
+      </c>
+      <c r="C62" s="9">
+        <v>64</v>
+      </c>
+      <c r="D62">
+        <v>320</v>
+      </c>
+      <c r="E62">
+        <v>168</v>
+      </c>
+      <c r="F62">
+        <v>212</v>
+      </c>
+      <c r="G62">
+        <v>159</v>
+      </c>
+      <c r="H62" s="9">
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+      <c r="J62">
+        <v>0</v>
+      </c>
+      <c r="K62">
+        <v>0</v>
+      </c>
+      <c r="L62">
+        <v>0</v>
+      </c>
+      <c r="M62">
+        <v>0</v>
+      </c>
+      <c r="N62">
+        <v>739</v>
+      </c>
+      <c r="O62">
+        <v>0</v>
+      </c>
+      <c r="P62">
+        <v>0</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17">
+      <c r="A63" t="s">
+        <v>230</v>
+      </c>
+      <c r="B63" t="s">
+        <v>202</v>
+      </c>
+      <c r="C63" s="9">
+        <v>64</v>
+      </c>
+      <c r="D63">
+        <v>320</v>
+      </c>
+      <c r="E63">
+        <v>168</v>
+      </c>
+      <c r="F63">
+        <v>212</v>
+      </c>
+      <c r="G63">
+        <v>159</v>
+      </c>
+      <c r="H63" s="9">
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+      <c r="J63">
+        <v>0</v>
+      </c>
+      <c r="K63">
+        <v>290</v>
+      </c>
+      <c r="L63">
+        <v>0</v>
+      </c>
+      <c r="M63">
+        <v>0</v>
+      </c>
+      <c r="N63">
+        <v>0</v>
+      </c>
+      <c r="O63">
+        <v>0</v>
+      </c>
+      <c r="P63">
+        <v>0</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17">
+      <c r="A64" t="s">
+        <v>230</v>
+      </c>
+      <c r="B64" t="s">
+        <v>204</v>
+      </c>
+      <c r="C64" s="9">
+        <v>64</v>
+      </c>
+      <c r="D64">
+        <v>320</v>
+      </c>
+      <c r="E64">
+        <v>168</v>
+      </c>
+      <c r="F64">
+        <v>212</v>
+      </c>
+      <c r="G64">
+        <v>159</v>
+      </c>
+      <c r="H64" s="9">
+        <v>37</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+      <c r="J64">
+        <v>0</v>
+      </c>
+      <c r="K64">
+        <v>533</v>
+      </c>
+      <c r="L64">
+        <v>0</v>
+      </c>
+      <c r="M64">
+        <v>0</v>
+      </c>
+      <c r="N64">
+        <v>0</v>
+      </c>
+      <c r="O64">
+        <v>0</v>
+      </c>
+      <c r="P64">
+        <v>0</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17">
+      <c r="A65" t="s">
+        <v>230</v>
+      </c>
+      <c r="B65" t="s">
+        <v>383</v>
+      </c>
+      <c r="C65" s="9">
+        <v>64</v>
+      </c>
+      <c r="D65">
+        <v>320</v>
+      </c>
+      <c r="E65">
+        <v>168</v>
+      </c>
+      <c r="F65">
+        <v>212</v>
+      </c>
+      <c r="G65">
+        <v>159</v>
+      </c>
+      <c r="H65" s="9">
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+      <c r="J65">
+        <v>0</v>
+      </c>
+      <c r="K65">
+        <v>0</v>
+      </c>
+      <c r="L65">
+        <v>0</v>
+      </c>
+      <c r="M65">
+        <v>0</v>
+      </c>
+      <c r="N65">
+        <v>761</v>
+      </c>
+      <c r="O65">
+        <v>0</v>
+      </c>
+      <c r="P65">
+        <v>0</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17">
+      <c r="A66" t="s">
+        <v>230</v>
+      </c>
+      <c r="B66" t="s">
+        <v>383</v>
+      </c>
+      <c r="C66" s="9">
+        <v>64</v>
+      </c>
+      <c r="D66">
+        <v>320</v>
+      </c>
+      <c r="E66">
+        <v>168</v>
+      </c>
+      <c r="F66">
+        <v>212</v>
+      </c>
+      <c r="G66">
+        <v>159</v>
+      </c>
+      <c r="H66" s="9">
+        <v>0</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
+      <c r="J66">
+        <v>0</v>
+      </c>
+      <c r="K66">
+        <v>0</v>
+      </c>
+      <c r="L66">
+        <v>0</v>
+      </c>
+      <c r="M66">
+        <v>212</v>
+      </c>
+      <c r="N66">
+        <v>0</v>
+      </c>
+      <c r="O66">
+        <v>0</v>
+      </c>
+      <c r="P66">
+        <v>0</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17">
+      <c r="A67" t="s">
+        <v>230</v>
+      </c>
+      <c r="B67" t="s">
+        <v>383</v>
+      </c>
+      <c r="C67" s="9">
+        <v>64</v>
+      </c>
+      <c r="D67">
+        <v>320</v>
+      </c>
+      <c r="E67">
+        <v>168</v>
+      </c>
+      <c r="F67">
+        <v>212</v>
+      </c>
+      <c r="G67">
+        <v>159</v>
+      </c>
+      <c r="H67" s="9">
+        <v>0</v>
+      </c>
+      <c r="I67">
+        <v>0</v>
+      </c>
+      <c r="J67">
+        <v>0</v>
+      </c>
+      <c r="K67">
+        <v>0</v>
+      </c>
+      <c r="L67">
+        <v>0</v>
+      </c>
+      <c r="M67">
+        <v>1360</v>
+      </c>
+      <c r="N67">
+        <v>761</v>
+      </c>
+      <c r="O67">
+        <v>0</v>
+      </c>
+      <c r="P67">
+        <v>0</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17">
+      <c r="A68" t="s">
+        <v>230</v>
+      </c>
+      <c r="B68" t="s">
+        <v>383</v>
+      </c>
+      <c r="C68" s="9">
+        <v>64</v>
+      </c>
+      <c r="D68">
+        <v>320</v>
+      </c>
+      <c r="E68">
+        <v>168</v>
+      </c>
+      <c r="F68">
+        <v>212</v>
+      </c>
+      <c r="G68">
+        <v>159</v>
+      </c>
+      <c r="H68" s="9">
+        <v>0</v>
+      </c>
+      <c r="I68">
+        <v>0</v>
+      </c>
+      <c r="J68">
+        <v>351</v>
+      </c>
+      <c r="K68">
+        <v>0</v>
+      </c>
+      <c r="L68">
+        <v>0</v>
+      </c>
+      <c r="M68">
+        <v>2010</v>
+      </c>
+      <c r="N68">
+        <v>0</v>
+      </c>
+      <c r="O68">
+        <v>0</v>
+      </c>
+      <c r="P68">
+        <v>1964</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17">
+      <c r="A69" t="s">
+        <v>230</v>
+      </c>
+      <c r="B69" t="s">
+        <v>388</v>
+      </c>
+      <c r="C69" s="9">
+        <v>64</v>
+      </c>
+      <c r="D69">
+        <v>320</v>
+      </c>
+      <c r="E69">
+        <v>168</v>
+      </c>
+      <c r="F69">
+        <v>212</v>
+      </c>
+      <c r="G69">
+        <v>159</v>
+      </c>
+      <c r="H69" s="9">
+        <v>53</v>
+      </c>
+      <c r="I69">
+        <v>0</v>
+      </c>
+      <c r="J69">
+        <v>0</v>
+      </c>
+      <c r="K69">
+        <v>497</v>
+      </c>
+      <c r="L69">
+        <v>0</v>
+      </c>
+      <c r="M69">
+        <v>0</v>
+      </c>
+      <c r="N69">
+        <v>0</v>
+      </c>
+      <c r="O69">
+        <v>0</v>
+      </c>
+      <c r="P69">
+        <v>0</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17">
+      <c r="A70" t="s">
+        <v>230</v>
+      </c>
+      <c r="B70" t="s">
+        <v>216</v>
+      </c>
+      <c r="C70" s="9">
+        <v>64</v>
+      </c>
+      <c r="D70">
+        <v>320</v>
+      </c>
+      <c r="E70">
+        <v>168</v>
+      </c>
+      <c r="F70">
+        <v>212</v>
+      </c>
+      <c r="G70">
+        <v>159</v>
+      </c>
+      <c r="H70" s="9">
+        <v>0</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+      <c r="J70">
+        <v>0</v>
+      </c>
+      <c r="K70">
+        <v>0</v>
+      </c>
+      <c r="L70">
+        <v>0</v>
+      </c>
+      <c r="M70">
         <v>221</v>
       </c>
-      <c r="M40">
-        <v>0</v>
-      </c>
-      <c r="N40" t="s">
+      <c r="N70">
+        <v>0</v>
+      </c>
+      <c r="O70">
+        <v>0</v>
+      </c>
+      <c r="P70">
+        <v>0</v>
+      </c>
+      <c r="Q70" t="s">
         <v>217</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17">
+      <c r="A71" t="s">
+        <v>230</v>
+      </c>
+      <c r="B71" t="s">
+        <v>390</v>
+      </c>
+      <c r="C71" s="9">
+        <v>64</v>
+      </c>
+      <c r="D71">
+        <v>320</v>
+      </c>
+      <c r="E71">
+        <v>168</v>
+      </c>
+      <c r="F71">
+        <v>212</v>
+      </c>
+      <c r="G71">
+        <v>159</v>
+      </c>
+      <c r="H71" s="9">
+        <v>0</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+      <c r="J71">
+        <v>0</v>
+      </c>
+      <c r="K71">
+        <v>0</v>
+      </c>
+      <c r="L71">
+        <v>0</v>
+      </c>
+      <c r="M71">
+        <v>0</v>
+      </c>
+      <c r="N71">
+        <v>0</v>
+      </c>
+      <c r="O71">
+        <v>200</v>
+      </c>
+      <c r="P71">
+        <v>0</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>391</v>
       </c>
     </row>
   </sheetData>

</xml_diff>